<commit_message>
#734 Got extraneous data warning test to pass by altering expression-sheet-parser.js.
</commit_message>
<xml_diff>
--- a/test-files/expression-data-test-sheets/expression_sheet_wrong_order_gene_names.xlsx
+++ b/test-files/expression-data-test-sheets/expression_sheet_wrong_order_gene_names.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\OneDrive\GRNsight\test-files\expression-data-test-sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Documents\GRNsight\test-files\expression-data-test-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C66127-5FC9-4872-97A4-E85487BD75B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794B5DB4-939B-472F-8B77-7AEB66E789B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wt_log2_expression" sheetId="6" r:id="rId1"/>
     <sheet name="network" sheetId="2" r:id="rId2"/>
-    <sheet name="network_weights" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>ACE2</t>
   </si>
@@ -1148,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1288,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1363,84 +1362,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>